<commit_message>
added combo for ded % loss and limit
</commit_message>
<xml_diff>
--- a/calc_rules.xlsx
+++ b/calc_rules.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF\oasislmf\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627DC94A-08DF-47E1-8802-72C4A3D27E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F8E71F-B5F0-4A04-A8D2-DE71BA019FF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calc_rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">calc_rules!$A$1:$M$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">calc_rules!$A$1:$M$95</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>desc</t>
   </si>
@@ -336,13 +336,25 @@
   </si>
   <si>
     <t>deductible with min deductible, no limit % TIV</t>
+  </si>
+  <si>
+    <t>no deductible; limit % TIV</t>
+  </si>
+  <si>
+    <t>no deductible % loss; limit % TIV</t>
+  </si>
+  <si>
+    <t>no deductible % TIV; limit % TIV</t>
+  </si>
+  <si>
+    <t>deductible % loss; limit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,6 +488,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -819,8 +837,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1176,13 +1195,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M89"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:M89"/>
+      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4859,7 +4878,7 @@
         <v>0</v>
       </c>
       <c r="M87" t="str">
-        <f t="shared" ref="M87:M89" si="6">"("&amp;C87&amp;", "&amp;D87&amp;", "&amp;E87&amp;", "&amp;F87&amp;", "&amp;G87&amp;", "&amp;H87&amp;", "&amp;I87&amp;", "&amp;J87&amp;", "&amp;K87&amp;", "&amp;L87&amp;")"</f>
+        <f t="shared" ref="M87:M93" si="6">"("&amp;C87&amp;", "&amp;D87&amp;", "&amp;E87&amp;", "&amp;F87&amp;", "&amp;G87&amp;", "&amp;H87&amp;", "&amp;I87&amp;", "&amp;J87&amp;", "&amp;K87&amp;", "&amp;L87&amp;")"</f>
         <v>(1, 1, 0, 0, 0, 0, 0, 0, 0, 0)</v>
       </c>
     </row>
@@ -4946,6 +4965,177 @@
         <f t="shared" si="6"/>
         <v>(1, 1, 0, 0, 0, 0, 0, 0, 2, 0)</v>
       </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90">
+        <v>14</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>2</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90" t="str">
+        <f t="shared" si="6"/>
+        <v>(0, 0, 0, 1, 0, 0, 0, 0, 2, 0)</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91">
+        <v>14</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>2</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91" t="str">
+        <f t="shared" si="6"/>
+        <v>(0, 0, 0, 1, 0, 0, 1, 0, 2, 0)</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92">
+        <v>14</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92">
+        <v>2</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>2</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92" t="str">
+        <f t="shared" si="6"/>
+        <v>(0, 0, 0, 1, 0, 0, 2, 0, 2, 0)</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>104</v>
+      </c>
+      <c r="B93">
+        <v>17</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93" t="str">
+        <f t="shared" si="6"/>
+        <v>(1, 0, 0, 1, 0, 0, 1, 0, 0, 0)</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>